<commit_message>
edit - removing the 3rd trial for pair 101
</commit_message>
<xml_diff>
--- a/analyses/pilotData_all_BY.xlsx
+++ b/analyses/pilotData_all_BY.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20396"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MMemeo\OneDrive - Fondazione Istituto Italiano Tecnologia\Documents\GitHub\joint-motor-decision\analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{DDF43D61-AFCC-4082-8C81-786064A4A95A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{7558693D-1004-4C8F-A8DE-BD6AF56C2B41}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{DDF43D61-AFCC-4082-8C81-786064A4A95A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{57AFF6BF-1842-437D-A58F-626A7E8C1F9B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13860" windowHeight="9330" activeTab="3" xr2:uid="{A80D8D59-C096-4587-A6C8-4C0B6ECCC775}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13860" windowHeight="9330" activeTab="1" xr2:uid="{A80D8D59-C096-4587-A6C8-4C0B6ECCC775}"/>
   </bookViews>
   <sheets>
     <sheet name="P100" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2050" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2047" uniqueCount="36">
   <si>
     <t>StimDuration</t>
   </si>
@@ -16939,10 +16939,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C94246B-2BAA-4FD1-82A3-919EB16CB05F}">
-  <dimension ref="A1:AH160"/>
+  <dimension ref="A1:AH159"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2:AB160"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Z159" sqref="Z159:AB159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17369,13 +17369,13 @@
         <v>3212</v>
       </c>
       <c r="Z4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC4" s="1">
         <v>0.51999998092651367</v>
@@ -17473,13 +17473,13 @@
         <v>3347</v>
       </c>
       <c r="Z5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC5" s="1">
         <v>0.64999997615814209</v>
@@ -17577,13 +17577,13 @@
         <v>5405</v>
       </c>
       <c r="Z6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC6" s="1">
         <v>0.57999998331069946</v>
@@ -17681,13 +17681,13 @@
         <v>1865</v>
       </c>
       <c r="Z7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC7" s="1">
         <v>1.0900000333786011</v>
@@ -17785,13 +17785,13 @@
         <v>3629</v>
       </c>
       <c r="Z8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC8" s="1">
         <v>0.69999998807907104</v>
@@ -17889,13 +17889,13 @@
         <v>1867</v>
       </c>
       <c r="Z9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC9" s="1">
         <v>1.1200000047683716</v>
@@ -17993,13 +17993,13 @@
         <v>3936</v>
       </c>
       <c r="Z10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC10" s="1">
         <v>0.47999998927116394</v>
@@ -18097,13 +18097,13 @@
         <v>1247</v>
       </c>
       <c r="Z11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC11" s="1">
         <v>0.95999997854232788</v>
@@ -18201,13 +18201,13 @@
         <v>4252</v>
       </c>
       <c r="Z12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC12" s="1">
         <v>0.37000000476837158</v>
@@ -18305,13 +18305,13 @@
         <v>1163</v>
       </c>
       <c r="Z13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC13" s="1">
         <v>0.40999999642372131</v>
@@ -18409,13 +18409,13 @@
         <v>3028</v>
       </c>
       <c r="Z14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AD14" s="1">
         <v>1.1399999856948853</v>
@@ -18507,13 +18507,13 @@
         <v>1892</v>
       </c>
       <c r="Z15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC15" s="1">
         <v>1.0399999618530273</v>
@@ -18611,13 +18611,13 @@
         <v>3577</v>
       </c>
       <c r="Z16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC16" s="1">
         <v>0.31000000238418579</v>
@@ -18715,13 +18715,13 @@
         <v>1078</v>
       </c>
       <c r="Z17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC17" s="1">
         <v>1.8300000429153442</v>
@@ -18819,13 +18819,13 @@
         <v>3215</v>
       </c>
       <c r="Z18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC18" s="1">
         <v>0.40999999642372131</v>
@@ -18923,13 +18923,13 @@
         <v>2015</v>
       </c>
       <c r="Z19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC19" s="1">
         <v>0.56999999284744263</v>
@@ -19027,13 +19027,13 @@
         <v>3407</v>
       </c>
       <c r="Z20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC20" s="1">
         <v>0.38999998569488525</v>
@@ -19131,13 +19131,13 @@
         <v>2990</v>
       </c>
       <c r="Z21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC21" s="1">
         <v>1.059999942779541</v>
@@ -19235,13 +19235,13 @@
         <v>3986</v>
       </c>
       <c r="Z22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC22" s="1">
         <v>0.55000001192092896</v>
@@ -19339,13 +19339,13 @@
         <v>1140</v>
       </c>
       <c r="Z23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC23" s="1">
         <v>1.1599999666213989</v>
@@ -19443,13 +19443,13 @@
         <v>2824</v>
       </c>
       <c r="Z24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC24" s="1">
         <v>0.36000001430511475</v>
@@ -19547,13 +19547,13 @@
         <v>802</v>
       </c>
       <c r="Z25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC25" s="1">
         <v>1.6299999952316284</v>
@@ -19651,13 +19651,13 @@
         <v>3739</v>
       </c>
       <c r="Z26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AD26" s="1">
         <v>2.130000114440918</v>
@@ -19749,13 +19749,13 @@
         <v>727</v>
       </c>
       <c r="Z27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC27" s="1">
         <v>0.52999997138977051</v>
@@ -19853,13 +19853,13 @@
         <v>3456</v>
       </c>
       <c r="Z28" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB28" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC28" s="1">
         <v>0.28999999165534973</v>
@@ -19957,13 +19957,13 @@
         <v>1831</v>
       </c>
       <c r="Z29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA29" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC29" s="1">
         <v>0.72000002861022949</v>
@@ -20061,13 +20061,13 @@
         <v>5066</v>
       </c>
       <c r="Z30" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB30" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC30" s="1">
         <v>0.36000001430511475</v>
@@ -20165,13 +20165,13 @@
         <v>1695</v>
       </c>
       <c r="Z31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA31" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC31" s="1">
         <v>0.85000002384185791</v>
@@ -20269,13 +20269,13 @@
         <v>5824</v>
       </c>
       <c r="Z32" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB32" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC32" s="1">
         <v>0.33000001311302185</v>
@@ -20373,13 +20373,13 @@
         <v>1802</v>
       </c>
       <c r="Z33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC33" s="1">
         <v>0.64999997615814209</v>
@@ -20477,13 +20477,13 @@
         <v>2564</v>
       </c>
       <c r="Z34" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB34" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC34" s="1">
         <v>2.559999942779541</v>
@@ -20581,13 +20581,13 @@
         <v>1937</v>
       </c>
       <c r="Z35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA35" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC35" s="1">
         <v>1.2200000286102295</v>
@@ -20685,13 +20685,13 @@
         <v>3970</v>
       </c>
       <c r="Z36" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB36" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC36" s="1">
         <v>0.36000001430511475</v>
@@ -20789,13 +20789,13 @@
         <v>820</v>
       </c>
       <c r="Z37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA37" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC37" s="1">
         <v>0.8399999737739563</v>
@@ -20893,13 +20893,13 @@
         <v>2215</v>
       </c>
       <c r="Z38" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB38" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC38" s="1">
         <v>0.37999999523162842</v>
@@ -20997,13 +20997,13 @@
         <v>1968</v>
       </c>
       <c r="Z39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA39" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC39" s="1">
         <v>0.87999999523162842</v>
@@ -21101,13 +21101,13 @@
         <v>2889</v>
       </c>
       <c r="Z40" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB40" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AD40" s="1">
         <v>1.309999942779541</v>
@@ -21199,13 +21199,13 @@
         <v>1981</v>
       </c>
       <c r="Z41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA41" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC41" s="1">
         <v>1.6699999570846558</v>
@@ -21303,13 +21303,13 @@
         <v>2668</v>
       </c>
       <c r="Z42" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB42" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AD42" s="1">
         <v>1.1699999570846558</v>
@@ -21401,13 +21401,13 @@
         <v>1623</v>
       </c>
       <c r="Z43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA43" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC43" s="1">
         <v>0.34000000357627869</v>
@@ -21505,13 +21505,13 @@
         <v>3128</v>
       </c>
       <c r="Z44" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB44" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC44" s="1">
         <v>0.68000000715255737</v>
@@ -21609,13 +21609,13 @@
         <v>1728</v>
       </c>
       <c r="Z45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA45" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC45" s="1">
         <v>1.8300000429153442</v>
@@ -21713,13 +21713,13 @@
         <v>2982</v>
       </c>
       <c r="Z46" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB46" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC46" s="1">
         <v>0.37999999523162842</v>
@@ -21817,13 +21817,13 @@
         <v>1750</v>
       </c>
       <c r="Z47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA47" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC47" s="1">
         <v>0.55000001192092896</v>
@@ -21921,13 +21921,13 @@
         <v>3625</v>
       </c>
       <c r="Z48" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB48" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC48" s="1">
         <v>0.37000000476837158</v>
@@ -22025,13 +22025,13 @@
         <v>929</v>
       </c>
       <c r="Z49" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA49" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB49" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AD49" s="1">
         <v>0.20999999344348907</v>
@@ -22123,13 +22123,13 @@
         <v>3372</v>
       </c>
       <c r="Z50" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA50" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB50" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC50" s="1">
         <v>0.34000000357627869</v>
@@ -22227,13 +22227,13 @@
         <v>1667</v>
       </c>
       <c r="Z51" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA51" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB51" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AD51" s="1">
         <v>0.40999999642372131</v>
@@ -22325,13 +22325,13 @@
         <v>1713</v>
       </c>
       <c r="Z52" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA52" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB52" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC52" s="1">
         <v>0.47999998927116394</v>
@@ -22429,13 +22429,13 @@
         <v>2055</v>
       </c>
       <c r="Z53" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA53" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB53" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC53" s="1">
         <v>1.5099999904632568</v>
@@ -22533,13 +22533,13 @@
         <v>2783</v>
       </c>
       <c r="Z54" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA54" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB54" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC54" s="1">
         <v>0.43000000715255737</v>
@@ -22637,13 +22637,13 @@
         <v>1231</v>
       </c>
       <c r="Z55" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA55" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB55" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC55" s="1">
         <v>0.73000001907348633</v>
@@ -22741,13 +22741,13 @@
         <v>2420</v>
       </c>
       <c r="Z56" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA56" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB56" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC56" s="1">
         <v>0.37999999523162842</v>
@@ -22845,13 +22845,13 @@
         <v>995</v>
       </c>
       <c r="Z57" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA57" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB57" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC57" s="1">
         <v>1.6499999761581421</v>
@@ -22949,13 +22949,13 @@
         <v>2150</v>
       </c>
       <c r="Z58" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA58" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB58" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC58" s="1">
         <v>0.60000002384185791</v>
@@ -23053,13 +23053,13 @@
         <v>921</v>
       </c>
       <c r="Z59" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA59" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB59" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC59" s="1">
         <v>2.4500000476837158</v>
@@ -23157,13 +23157,13 @@
         <v>2005</v>
       </c>
       <c r="Z60" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA60" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB60" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC60" s="1">
         <v>0.33000001311302185</v>
@@ -23255,13 +23255,13 @@
         <v>874</v>
       </c>
       <c r="Z61" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA61" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB61" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC61" s="1">
         <v>1.3999999761581421</v>
@@ -23359,13 +23359,13 @@
         <v>2333</v>
       </c>
       <c r="Z62" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA62" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB62" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC62" s="1">
         <v>0.34000000357627869</v>
@@ -23463,13 +23463,13 @@
         <v>814</v>
       </c>
       <c r="Z63" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA63" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB63" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC63" s="1">
         <v>1.309999942779541</v>
@@ -23561,13 +23561,13 @@
         <v>2552</v>
       </c>
       <c r="Z64" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA64" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB64" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC64" s="1">
         <v>0.33000001311302185</v>
@@ -23665,13 +23665,13 @@
         <v>1696</v>
       </c>
       <c r="Z65" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA65" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB65" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC65" s="1">
         <v>1.309999942779541</v>
@@ -23763,13 +23763,13 @@
         <v>3307</v>
       </c>
       <c r="Z66" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA66" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB66" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AD66" s="1">
         <v>2.0799999237060547</v>
@@ -23861,13 +23861,13 @@
         <v>1045</v>
       </c>
       <c r="Z67" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA67" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB67" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC67" s="1">
         <v>0.47999998927116394</v>
@@ -23965,13 +23965,13 @@
         <v>4858</v>
       </c>
       <c r="Z68" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA68" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB68" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC68" s="1">
         <v>0.36000001430511475</v>
@@ -24069,13 +24069,13 @@
         <v>1936</v>
       </c>
       <c r="Z69" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA69" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB69" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC69" s="1">
         <v>0.49000000953674316</v>
@@ -24173,13 +24173,13 @@
         <v>2129</v>
       </c>
       <c r="Z70" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA70" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB70" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC70" s="1">
         <v>0.36000001430511475</v>
@@ -24277,13 +24277,13 @@
         <v>710</v>
       </c>
       <c r="Z71" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA71" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB71" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC71" s="1">
         <v>1.4800000190734863</v>
@@ -24381,13 +24381,13 @@
         <v>2323</v>
       </c>
       <c r="Z72" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA72" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB72" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC72" s="1">
         <v>0.4699999988079071</v>
@@ -24485,13 +24485,13 @@
         <v>2262</v>
       </c>
       <c r="Z73" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA73" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB73" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC73" s="1">
         <v>0.49000000953674316</v>
@@ -24583,13 +24583,13 @@
         <v>2605</v>
       </c>
       <c r="Z74" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA74" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB74" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AD74" s="1">
         <v>3.869999885559082</v>
@@ -24675,13 +24675,13 @@
         <v>1642</v>
       </c>
       <c r="Z75" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA75" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB75" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC75" s="1">
         <v>0.55000001192092896</v>
@@ -24779,13 +24779,13 @@
         <v>3018</v>
       </c>
       <c r="Z76" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA76" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB76" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC76" s="1">
         <v>0.36000001430511475</v>
@@ -24883,13 +24883,13 @@
         <v>1095</v>
       </c>
       <c r="Z77" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA77" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB77" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC77" s="1">
         <v>0.49000000953674316</v>
@@ -24987,13 +24987,13 @@
         <v>3065</v>
       </c>
       <c r="Z78" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA78" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB78" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AD78" s="1">
         <v>0.62000000476837158</v>
@@ -25085,13 +25085,13 @@
         <v>2593</v>
       </c>
       <c r="Z79" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA79" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB79" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC79" s="1">
         <v>0.68999999761581421</v>
@@ -25189,13 +25189,13 @@
         <v>2003</v>
       </c>
       <c r="Z80" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA80" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB80" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC80" s="1">
         <v>0.33000001311302185</v>
@@ -25287,13 +25287,13 @@
         <v>1384</v>
       </c>
       <c r="Z81" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA81" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB81" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC81" s="1">
         <v>0.61000001430511475</v>
@@ -25391,13 +25391,13 @@
         <v>2340</v>
       </c>
       <c r="Z82" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA82" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB82" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC82" s="1">
         <v>0.28999999165534973</v>
@@ -25495,13 +25495,13 @@
         <v>996</v>
       </c>
       <c r="Z83" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA83" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB83" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC83" s="1">
         <v>0.77999997138977051</v>
@@ -25599,13 +25599,13 @@
         <v>2156</v>
       </c>
       <c r="Z84" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA84" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB84" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AD84" s="1">
         <v>0.50999999046325684</v>
@@ -25697,13 +25697,13 @@
         <v>746</v>
       </c>
       <c r="Z85" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA85" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB85" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC85" s="1">
         <v>0.82999998331069946</v>
@@ -25801,13 +25801,13 @@
         <v>1611</v>
       </c>
       <c r="Z86" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA86" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB86" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC86" s="1">
         <v>0.27000001072883606</v>
@@ -25905,13 +25905,13 @@
         <v>2824</v>
       </c>
       <c r="Z87" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA87" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB87" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC87" s="1">
         <v>0.92000001668930054</v>
@@ -26009,13 +26009,13 @@
         <v>2939</v>
       </c>
       <c r="Z88" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA88" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB88" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AD88" s="1">
         <v>0.34999999403953552</v>
@@ -26107,13 +26107,13 @@
         <v>1000</v>
       </c>
       <c r="Z89" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA89" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB89" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC89" s="1">
         <v>0.54000002145767212</v>
@@ -26211,13 +26211,13 @@
         <v>1825</v>
       </c>
       <c r="Z90" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA90" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB90" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC90" s="1">
         <v>0.4699999988079071</v>
@@ -26315,13 +26315,13 @@
         <v>932.99999999953434</v>
       </c>
       <c r="Z91" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA91" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB91" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AD91" s="1">
         <v>0.18999999761581421</v>
@@ -26413,13 +26413,13 @@
         <v>2204.0000000004657</v>
       </c>
       <c r="Z92" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA92" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB92" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC92" s="1">
         <v>0.38999998569488525</v>
@@ -26517,13 +26517,13 @@
         <v>703.00000000046566</v>
       </c>
       <c r="Z93" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA93" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB93" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AD93" s="1">
         <v>0.27000001072883606</v>
@@ -26615,13 +26615,13 @@
         <v>2350</v>
       </c>
       <c r="Z94" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA94" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB94" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC94" s="1">
         <v>0.34999999403953552</v>
@@ -26719,13 +26719,13 @@
         <v>1361</v>
       </c>
       <c r="Z95" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA95" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB95" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC95" s="1">
         <v>0.46000000834465027</v>
@@ -26823,13 +26823,13 @@
         <v>1292</v>
       </c>
       <c r="Z96" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA96" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB96" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC96" s="1">
         <v>0.54000002145767212</v>
@@ -26927,13 +26927,13 @@
         <v>1261</v>
       </c>
       <c r="Z97" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA97" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB97" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AD97" s="1">
         <v>0.77999997138977051</v>
@@ -27025,13 +27025,13 @@
         <v>3431</v>
       </c>
       <c r="Z98" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA98" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB98" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC98" s="1">
         <v>0.41999998688697815</v>
@@ -27129,13 +27129,13 @@
         <v>884</v>
       </c>
       <c r="Z99" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA99" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB99" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AD99" s="1">
         <v>0.37000000476837158</v>
@@ -27227,13 +27227,13 @@
         <v>3123</v>
       </c>
       <c r="Z100" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA100" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB100" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC100" s="1">
         <v>0.51999998092651367</v>
@@ -27331,13 +27331,13 @@
         <v>847</v>
       </c>
       <c r="Z101" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA101" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB101" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC101" s="1">
         <v>0.5899999737739563</v>
@@ -27435,13 +27435,13 @@
         <v>4233</v>
       </c>
       <c r="Z102" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA102" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB102" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC102" s="1">
         <v>0.31000000238418579</v>
@@ -27539,13 +27539,13 @@
         <v>1339</v>
       </c>
       <c r="Z103" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA103" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB103" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC103" s="1">
         <v>0.2800000011920929</v>
@@ -27637,13 +27637,13 @@
         <v>3169</v>
       </c>
       <c r="Z104" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA104" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB104" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC104" s="1">
         <v>0.30000001192092896</v>
@@ -27741,13 +27741,13 @@
         <v>1169</v>
       </c>
       <c r="Z105" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA105" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB105" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC105" s="1">
         <v>1.2100000381469727</v>
@@ -27839,13 +27839,13 @@
         <v>3027</v>
       </c>
       <c r="Z106" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA106" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB106" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC106" s="1">
         <v>0.40999999642372131</v>
@@ -27937,13 +27937,13 @@
         <v>2555</v>
       </c>
       <c r="Z107" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA107" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB107" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC107" s="1">
         <v>1.1200000047683716</v>
@@ -28041,13 +28041,13 @@
         <v>3231</v>
       </c>
       <c r="Z108" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA108" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB108" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC108" s="1">
         <v>0.43000000715255737</v>
@@ -28145,13 +28145,13 @@
         <v>1881</v>
       </c>
       <c r="Z109" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA109" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB109" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC109" s="1">
         <v>0.75999999046325684</v>
@@ -28249,13 +28249,13 @@
         <v>2473</v>
       </c>
       <c r="Z110" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA110" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB110" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC110" s="1">
         <v>0.31000000238418579</v>
@@ -28353,13 +28353,13 @@
         <v>1655</v>
       </c>
       <c r="Z111" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA111" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB111" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC111" s="1">
         <v>0.43000000715255737</v>
@@ -28457,13 +28457,13 @@
         <v>3338</v>
       </c>
       <c r="Z112" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA112" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB112" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC112" s="1">
         <v>0.43999999761581421</v>
@@ -28561,13 +28561,13 @@
         <v>911</v>
       </c>
       <c r="Z113" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA113" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB113" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC113" s="1">
         <v>0.49000000953674316</v>
@@ -28659,13 +28659,13 @@
         <v>4121</v>
       </c>
       <c r="Z114" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA114" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB114" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC114" s="1">
         <v>0.27000001072883606</v>
@@ -28763,13 +28763,13 @@
         <v>1661</v>
       </c>
       <c r="Z115" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA115" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB115" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC115" s="1">
         <v>0.47999998927116394</v>
@@ -28867,13 +28867,13 @@
         <v>3293</v>
       </c>
       <c r="Z116" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA116" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB116" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AD116" s="1">
         <v>3.309999942779541</v>
@@ -28965,13 +28965,13 @@
         <v>1370</v>
       </c>
       <c r="Z117" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA117" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB117" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC117" s="1">
         <v>0.99000000953674316</v>
@@ -29069,13 +29069,13 @@
         <v>1463</v>
       </c>
       <c r="Z118" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA118" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB118" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC118" s="1">
         <v>0.49000000953674316</v>
@@ -29173,13 +29173,13 @@
         <v>927</v>
       </c>
       <c r="Z119" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA119" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB119" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC119" s="1">
         <v>1.809999942779541</v>
@@ -29277,13 +29277,13 @@
         <v>2665</v>
       </c>
       <c r="Z120" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA120" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB120" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC120" s="1">
         <v>2.0999999046325684</v>
@@ -29381,13 +29381,13 @@
         <v>878</v>
       </c>
       <c r="Z121" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA121" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB121" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC121" s="1">
         <v>0.46000000834465027</v>
@@ -29485,13 +29485,13 @@
         <v>2527</v>
       </c>
       <c r="Z122" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA122" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB122" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC122" s="1">
         <v>0.41999998688697815</v>
@@ -29589,13 +29589,13 @@
         <v>805</v>
       </c>
       <c r="Z123" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA123" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB123" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC123" s="1">
         <v>1.1299999952316284</v>
@@ -29693,13 +29693,13 @@
         <v>1457</v>
       </c>
       <c r="Z124" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA124" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB124" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC124" s="1">
         <v>0.68999999761581421</v>
@@ -29797,13 +29797,13 @@
         <v>622</v>
       </c>
       <c r="Z125" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA125" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB125" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC125" s="1">
         <v>1.0800000429153442</v>
@@ -29901,13 +29901,13 @@
         <v>1792</v>
       </c>
       <c r="Z126" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA126" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB126" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC126" s="1">
         <v>0.63999998569488525</v>
@@ -30005,13 +30005,13 @@
         <v>1255</v>
       </c>
       <c r="Z127" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA127" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB127" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC127" s="1">
         <v>0.87999999523162842</v>
@@ -30109,13 +30109,13 @@
         <v>2572</v>
       </c>
       <c r="Z128" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA128" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB128" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC128" s="1">
         <v>0.46000000834465027</v>
@@ -30207,13 +30207,13 @@
         <v>514</v>
       </c>
       <c r="Z129" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA129" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB129" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC129" s="1">
         <v>0.69999998807907104</v>
@@ -30311,13 +30311,13 @@
         <v>2742</v>
       </c>
       <c r="Z130" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA130" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB130" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC130" s="1">
         <v>0.34000000357627869</v>
@@ -30415,13 +30415,13 @@
         <v>722</v>
       </c>
       <c r="Z131" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA131" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB131" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC131" s="1">
         <v>0.50999999046325684</v>
@@ -30519,13 +30519,13 @@
         <v>2559</v>
       </c>
       <c r="Z132" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA132" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB132" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC132" s="1">
         <v>0.27000001072883606</v>
@@ -30617,13 +30617,13 @@
         <v>380</v>
       </c>
       <c r="Z133" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA133" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB133" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC133" s="1">
         <v>0.88999998569488525</v>
@@ -30721,13 +30721,13 @@
         <v>1950</v>
       </c>
       <c r="Z134" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA134" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB134" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AD134" s="1">
         <v>0.8399999737739563</v>
@@ -30819,13 +30819,13 @@
         <v>1139</v>
       </c>
       <c r="Z135" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA135" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB135" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC135" s="1">
         <v>0.44999998807907104</v>
@@ -30917,13 +30917,13 @@
         <v>2617</v>
       </c>
       <c r="Z136" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA136" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB136" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC136" s="1">
         <v>0.4699999988079071</v>
@@ -31021,13 +31021,13 @@
         <v>687</v>
       </c>
       <c r="Z137" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA137" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB137" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC137" s="1">
         <v>0.47999998927116394</v>
@@ -31125,13 +31125,13 @@
         <v>4114</v>
       </c>
       <c r="Z138" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA138" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB138" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC138" s="1">
         <v>0.34000000357627869</v>
@@ -31229,13 +31229,13 @@
         <v>1117</v>
       </c>
       <c r="Z139" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA139" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB139" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC139" s="1">
         <v>0.68000000715255737</v>
@@ -31327,13 +31327,13 @@
         <v>3340</v>
       </c>
       <c r="Z140" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA140" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB140" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC140" s="1">
         <v>0.20999999344348907</v>
@@ -31431,13 +31431,13 @@
         <v>1505</v>
       </c>
       <c r="Z141" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA141" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB141" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC141" s="1">
         <v>0.97000002861022949</v>
@@ -31535,13 +31535,13 @@
         <v>2839</v>
       </c>
       <c r="Z142" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA142" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB142" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC142" s="1">
         <v>0.23999999463558197</v>
@@ -31639,13 +31639,13 @@
         <v>615</v>
       </c>
       <c r="Z143" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA143" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB143" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC143" s="1">
         <v>0.27000001072883606</v>
@@ -31743,13 +31743,13 @@
         <v>4646</v>
       </c>
       <c r="Z144" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA144" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB144" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC144" s="1">
         <v>0.23000000417232513</v>
@@ -31841,13 +31841,13 @@
         <v>712</v>
       </c>
       <c r="Z145" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA145" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB145" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC145" s="1">
         <v>1.2400000095367432</v>
@@ -31945,13 +31945,13 @@
         <v>2872</v>
       </c>
       <c r="Z146" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA146" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB146" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC146" s="1">
         <v>0.30000001192092896</v>
@@ -32049,13 +32049,13 @@
         <v>886</v>
       </c>
       <c r="Z147" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA147" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB147" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC147" s="1">
         <v>0.56999999284744263</v>
@@ -32153,13 +32153,13 @@
         <v>1766</v>
       </c>
       <c r="Z148" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA148" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB148" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC148" s="1">
         <v>0.36000001430511475</v>
@@ -32251,13 +32251,13 @@
         <v>1050</v>
       </c>
       <c r="Z149" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA149" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB149" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC149" s="1">
         <v>0.41999998688697815</v>
@@ -32355,13 +32355,13 @@
         <v>1880</v>
       </c>
       <c r="Z150" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA150" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB150" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC150" s="1">
         <v>0.34999999403953552</v>
@@ -32459,13 +32459,13 @@
         <v>810</v>
       </c>
       <c r="Z151" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA151" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB151" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC151" s="1">
         <v>1.0700000524520874</v>
@@ -32563,13 +32563,13 @@
         <v>2551</v>
       </c>
       <c r="Z152" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA152" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB152" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC152" s="1">
         <v>0.34000000357627869</v>
@@ -32667,13 +32667,13 @@
         <v>1202</v>
       </c>
       <c r="Z153" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA153" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB153" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC153" s="1">
         <v>0.50999999046325684</v>
@@ -32765,13 +32765,13 @@
         <v>2555</v>
       </c>
       <c r="Z154" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA154" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB154" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC154" s="1">
         <v>0.27000001072883606</v>
@@ -32869,13 +32869,13 @@
         <v>781</v>
       </c>
       <c r="Z155" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA155" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB155" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC155" s="1">
         <v>0.49000000953674316</v>
@@ -32973,13 +32973,13 @@
         <v>3372</v>
       </c>
       <c r="Z156" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA156" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB156" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC156" s="1">
         <v>0.33000001311302185</v>
@@ -33077,13 +33077,13 @@
         <v>876</v>
       </c>
       <c r="Z157" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA157" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB157" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC157" s="1">
         <v>1.1200000047683716</v>
@@ -33181,13 +33181,13 @@
         <v>3143</v>
       </c>
       <c r="Z158" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA158" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB158" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC158" s="1">
         <v>0.25999999046325684</v>
@@ -33278,14 +33278,14 @@
       <c r="Y159">
         <v>1298</v>
       </c>
-      <c r="Z159" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA159" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB159" t="s">
-        <v>35</v>
+      <c r="Z159" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA159" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB159" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="AC159" s="1">
         <v>0.68999999761581421</v>
@@ -33304,104 +33304,6 @@
       </c>
       <c r="AH159" s="1">
         <v>2.7000000476837158</v>
-      </c>
-    </row>
-    <row r="160" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A160">
-        <v>85</v>
-      </c>
-      <c r="B160">
-        <v>1</v>
-      </c>
-      <c r="C160">
-        <v>0.1</v>
-      </c>
-      <c r="D160">
-        <v>0.15</v>
-      </c>
-      <c r="E160">
-        <v>0.25</v>
-      </c>
-      <c r="F160">
-        <v>2</v>
-      </c>
-      <c r="G160">
-        <v>1</v>
-      </c>
-      <c r="H160">
-        <v>2</v>
-      </c>
-      <c r="I160">
-        <v>1</v>
-      </c>
-      <c r="J160">
-        <v>12</v>
-      </c>
-      <c r="K160">
-        <v>623</v>
-      </c>
-      <c r="L160">
-        <v>2</v>
-      </c>
-      <c r="M160">
-        <v>733</v>
-      </c>
-      <c r="N160">
-        <v>2</v>
-      </c>
-      <c r="O160">
-        <v>1</v>
-      </c>
-      <c r="P160">
-        <v>533</v>
-      </c>
-      <c r="Q160">
-        <v>655</v>
-      </c>
-      <c r="R160">
-        <v>3</v>
-      </c>
-      <c r="S160">
-        <v>2309</v>
-      </c>
-      <c r="T160">
-        <v>2</v>
-      </c>
-      <c r="U160">
-        <v>1</v>
-      </c>
-      <c r="V160">
-        <v>1110</v>
-      </c>
-      <c r="W160">
-        <v>471</v>
-      </c>
-      <c r="X160">
-        <v>6</v>
-      </c>
-      <c r="Y160">
-        <v>3316</v>
-      </c>
-      <c r="Z160" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA160" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB160" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC160" s="1">
-        <v>0.37999999523162842</v>
-      </c>
-      <c r="AD160" s="1">
-        <v>0.43000000715255737</v>
-      </c>
-      <c r="AF160" s="1">
-        <v>0.63999998569488525</v>
-      </c>
-      <c r="AG160" s="1">
-        <v>0.75999999046325684</v>
       </c>
     </row>
   </sheetData>
@@ -49752,7 +49654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62958CC0-5403-4412-9F7C-A43A58ADDD35}">
   <dimension ref="A1:AH161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="Z2" sqref="Z2:AB161"/>
     </sheetView>
   </sheetViews>
@@ -66593,17 +66495,17 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4CE8736-71CD-443B-A535-A7744CB96E37}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="23934a0c-d8ba-4782-9c92-a3b70815aabd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ce182090-6989-4ee1-a763-8685359d9a12"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="23934a0c-d8ba-4782-9c92-a3b70815aabd"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ce182090-6989-4ee1-a763-8685359d9a12"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>